<commit_message>
my b did a lot
</commit_message>
<xml_diff>
--- a/lib/MenuPage/menus/Bar 1.xlsx
+++ b/lib/MenuPage/menus/Bar 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chide/Desktop/barzzy_app2/lib/MenuPage/menus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB6FB2B-4C95-0B40-8853-A091F4939BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADC6485-3119-2F47-8196-FCA0202E4AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{FA48C04F-F26E-274D-B83D-EDD113380032}"/>
+    <workbookView xWindow="29400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{FA48C04F-F26E-274D-B83D-EDD113380032}"/>
   </bookViews>
   <sheets>
     <sheet name="The Burg" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="94">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>Classc</t>
+  </si>
+  <si>
+    <t>Selzter</t>
+  </si>
+  <si>
+    <t>Sezlter</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -767,7 +773,7 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,15 +810,15 @@
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
@@ -822,11 +828,11 @@
       <c r="J2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="5"/>
@@ -839,15 +845,15 @@
       <c r="B3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
       <c r="H3" s="2">
         <v>8.99</v>
       </c>
@@ -869,11 +875,11 @@
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -885,15 +891,15 @@
       <c r="B4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="2">
         <v>9.99</v>
       </c>
@@ -915,11 +921,11 @@
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
       <c r="V4" s="2"/>
       <c r="W4" s="3"/>
       <c r="X4" s="7"/>
@@ -931,15 +937,15 @@
       <c r="B5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="2">
         <v>7.99</v>
       </c>
@@ -961,11 +967,11 @@
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
       <c r="V5" s="2"/>
       <c r="W5" s="3"/>
       <c r="X5" s="7"/>
@@ -977,15 +983,15 @@
       <c r="B6" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="2">
         <v>6.99</v>
       </c>
@@ -1007,11 +1013,11 @@
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
       <c r="V6" s="2"/>
       <c r="W6" s="3"/>
       <c r="X6" s="7"/>
@@ -1023,15 +1029,15 @@
       <c r="B7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="2">
         <v>8.99</v>
       </c>
@@ -1053,11 +1059,11 @@
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="2"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
       <c r="V7" s="2"/>
       <c r="W7" s="3"/>
       <c r="X7" s="7"/>
@@ -1069,15 +1075,15 @@
       <c r="B8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="2">
         <v>3.99</v>
       </c>
@@ -1099,11 +1105,11 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="2"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
       <c r="V8" s="2"/>
       <c r="W8" s="3"/>
       <c r="X8" s="7"/>
@@ -1115,15 +1121,15 @@
       <c r="B9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="2">
         <v>9.99</v>
       </c>
@@ -1139,15 +1145,17 @@
       <c r="L9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="6"/>
+      <c r="M9" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="2"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
       <c r="V9" s="2"/>
       <c r="W9" s="3"/>
       <c r="X9" s="7"/>
@@ -1159,15 +1167,15 @@
       <c r="B10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="2">
         <v>10.99</v>
       </c>
@@ -1189,11 +1197,11 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
       <c r="V10" s="2"/>
       <c r="W10" s="3"/>
       <c r="X10" s="7"/>
@@ -1205,15 +1213,15 @@
       <c r="B11" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="2">
         <v>14.99</v>
       </c>
@@ -1229,15 +1237,17 @@
       <c r="L11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M11" s="6"/>
+      <c r="M11" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="2"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
       <c r="V11" s="2"/>
       <c r="W11" s="3"/>
       <c r="X11" s="7"/>
@@ -1249,15 +1259,15 @@
       <c r="B12" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="2">
         <v>3.99</v>
       </c>
@@ -1279,11 +1289,11 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="2"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
       <c r="V12" s="2"/>
       <c r="W12" s="3"/>
       <c r="X12" s="7"/>
@@ -1295,15 +1305,15 @@
       <c r="B13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="2">
         <v>6.99</v>
       </c>
@@ -1325,11 +1335,11 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
       <c r="V13" s="2"/>
       <c r="W13" s="3"/>
       <c r="X13" s="7"/>
@@ -1341,15 +1351,15 @@
       <c r="B14" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="2">
         <v>4.99</v>
       </c>
@@ -1371,11 +1381,11 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="2"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
       <c r="V14" s="2"/>
       <c r="W14" s="3"/>
       <c r="X14" s="7"/>
@@ -1387,15 +1397,15 @@
       <c r="B15" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="2">
         <v>4.99</v>
       </c>
@@ -1417,11 +1427,11 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="2"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
       <c r="V15" s="2"/>
       <c r="W15" s="3"/>
       <c r="X15" s="7"/>
@@ -1433,15 +1443,15 @@
       <c r="B16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="2">
         <v>4.99</v>
       </c>
@@ -1463,11 +1473,11 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="2"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
       <c r="V16" s="2"/>
       <c r="W16" s="3"/>
       <c r="X16" s="7"/>
@@ -1479,15 +1489,15 @@
       <c r="B17" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="2">
         <v>4.99</v>
       </c>
@@ -1503,15 +1513,17 @@
       <c r="L17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M17" s="6"/>
+      <c r="M17" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="2"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
       <c r="V17" s="2"/>
       <c r="W17" s="3"/>
       <c r="X17" s="7"/>
@@ -1523,15 +1535,15 @@
       <c r="B18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="2">
         <v>4.99</v>
       </c>
@@ -1553,11 +1565,11 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="2"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
       <c r="V18" s="2"/>
       <c r="W18" s="3"/>
       <c r="X18" s="7"/>
@@ -1569,15 +1581,15 @@
       <c r="B19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="2">
         <v>4.99</v>
       </c>
@@ -1593,15 +1605,17 @@
       <c r="L19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="6"/>
+      <c r="M19" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="2"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
       <c r="V19" s="2"/>
       <c r="W19" s="3"/>
       <c r="X19" s="7"/>
@@ -1613,15 +1627,15 @@
       <c r="B20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="2">
         <v>4.99</v>
       </c>
@@ -1643,11 +1657,11 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="2"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
       <c r="V20" s="2"/>
       <c r="W20" s="3"/>
       <c r="X20" s="7"/>
@@ -1659,15 +1673,15 @@
       <c r="B21" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="2">
         <v>4.99</v>
       </c>
@@ -1689,11 +1703,11 @@
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="2"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
       <c r="V21" s="2"/>
       <c r="W21" s="3"/>
       <c r="X21" s="7"/>
@@ -1705,15 +1719,15 @@
       <c r="B22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="2">
         <v>4.99</v>
       </c>
@@ -1735,11 +1749,11 @@
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="2"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
       <c r="V22" s="2"/>
       <c r="W22" s="3"/>
       <c r="X22" s="7"/>
@@ -1751,15 +1765,15 @@
       <c r="B23" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="2">
         <v>4.99</v>
       </c>
@@ -1781,11 +1795,11 @@
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="2"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
       <c r="V23" s="2"/>
       <c r="W23" s="3"/>
       <c r="X23" s="7"/>
@@ -1797,15 +1811,15 @@
       <c r="B24" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8" t="s">
+      <c r="D24" s="9"/>
+      <c r="E24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="2">
         <v>4.99</v>
       </c>
@@ -1827,11 +1841,11 @@
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="2"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
       <c r="V24" s="2"/>
       <c r="W24" s="3"/>
       <c r="X24" s="7"/>
@@ -1843,15 +1857,15 @@
       <c r="B25" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8" t="s">
+      <c r="D25" s="9"/>
+      <c r="E25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="2">
         <v>4.99</v>
       </c>
@@ -1873,11 +1887,11 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="2"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
       <c r="V25" s="2"/>
       <c r="W25" s="3"/>
       <c r="X25" s="7"/>
@@ -1889,15 +1903,15 @@
       <c r="B26" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8" t="s">
+      <c r="D26" s="9"/>
+      <c r="E26" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="2">
         <v>4.99</v>
       </c>
@@ -1919,11 +1933,11 @@
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="2"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
       <c r="V26" s="2"/>
       <c r="W26" s="3"/>
       <c r="X26" s="7"/>
@@ -1935,15 +1949,15 @@
       <c r="B27" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="9"/>
+      <c r="E27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
       <c r="H27" s="2">
         <v>4.99</v>
       </c>
@@ -1965,11 +1979,11 @@
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="2"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="8"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
       <c r="V27" s="2"/>
       <c r="W27" s="3"/>
       <c r="X27" s="7"/>
@@ -1981,15 +1995,15 @@
       <c r="B28" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8" t="s">
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
       <c r="H28" s="2">
         <v>4.99</v>
       </c>
@@ -2011,11 +2025,11 @@
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="2"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
       <c r="V28" s="2"/>
       <c r="W28" s="3"/>
       <c r="X28" s="7"/>
@@ -2027,15 +2041,15 @@
       <c r="B29" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8" t="s">
+      <c r="D29" s="9"/>
+      <c r="E29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
       <c r="H29" s="2">
         <v>4.99</v>
       </c>
@@ -2051,15 +2065,17 @@
       <c r="L29" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M29" s="6"/>
+      <c r="M29" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="2"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
       <c r="V29" s="2"/>
       <c r="W29" s="3"/>
       <c r="X29" s="7"/>
@@ -2071,15 +2087,15 @@
       <c r="B30" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8" t="s">
+      <c r="D30" s="9"/>
+      <c r="E30" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
       <c r="H30" s="2">
         <v>4.99</v>
       </c>
@@ -2101,11 +2117,11 @@
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="2"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
       <c r="V30" s="2"/>
       <c r="W30" s="3"/>
       <c r="X30" s="7"/>
@@ -2117,15 +2133,15 @@
       <c r="B31" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8" t="s">
+      <c r="D31" s="9"/>
+      <c r="E31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
       <c r="H31" s="2">
         <v>4.99</v>
       </c>
@@ -2141,15 +2157,17 @@
       <c r="L31" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M31" s="6"/>
+      <c r="M31" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="2"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
       <c r="V31" s="2"/>
       <c r="W31" s="3"/>
       <c r="X31" s="7"/>
@@ -2164,11 +2182,11 @@
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="2"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
       <c r="V32" s="2"/>
       <c r="W32" s="3"/>
       <c r="X32" s="7"/>
@@ -2275,6 +2293,106 @@
     </row>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="S19:U19"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="S31:U31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="S32:U32"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="S29:U29"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="S30:U30"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="S25:U25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:G22"/>
@@ -2299,106 +2417,6 @@
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="S30:U30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="S31:U31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="S32:U32"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="S29:U29"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="S25:U25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="S19:U19"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>